<commit_message>
add after stop interrupt source and tested
</commit_message>
<xml_diff>
--- a/doc/XBR820  system spec/xbr820_register.xlsx
+++ b/doc/XBR820  system spec/xbr820_register.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\XBR820\Document\Register\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D009F694-4FDE-46AA-81F2-18C95B4F9678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="12578" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MemMap" sheetId="20" r:id="rId1"/>
@@ -24,9 +18,9 @@
     <sheet name="flash" sheetId="18" r:id="rId9"/>
     <sheet name="interrupts" sheetId="21" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="961">
   <si>
     <t>RO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3869,12 +3863,26 @@
     <t>IO triger mode  1:over threshold triger  0:time meet triger</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>stop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>之后立起来</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4055,6 +4063,11 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="等线"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -4375,7 +4388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4690,16 +4703,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4714,38 +4760,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4807,7 +4823,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -4842,7 +4858,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -5019,31 +5035,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EB3F28-8067-4A17-9578-304DE1B9D9E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="38.109375" customWidth="1"/>
+    <col min="6" max="6" width="38.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1">
+    <row r="1" spans="1:6" ht="15.4" thickBot="1">
       <c r="A1" s="62" t="s">
         <v>663</v>
       </c>
@@ -5063,7 +5079,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" thickBot="1">
+    <row r="2" spans="1:6" ht="15.4" thickBot="1">
       <c r="A2" s="65" t="s">
         <v>669</v>
       </c>
@@ -5083,7 +5099,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" thickBot="1">
+    <row r="3" spans="1:6" ht="15.4" thickBot="1">
       <c r="A3" s="65" t="s">
         <v>675</v>
       </c>
@@ -5231,7 +5247,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" thickBot="1">
+    <row r="11" spans="1:6" ht="15.4" thickBot="1">
       <c r="A11" s="106"/>
       <c r="B11" s="75" t="s">
         <v>712</v>
@@ -5355,7 +5371,7 @@
       <c r="E18" s="77"/>
       <c r="F18" s="78"/>
     </row>
-    <row r="19" spans="1:6" ht="15.6" thickBot="1">
+    <row r="19" spans="1:6" ht="15.4" thickBot="1">
       <c r="A19" s="106"/>
       <c r="B19" s="79" t="s">
         <v>731</v>
@@ -5369,7 +5385,7 @@
       <c r="E19" s="79"/>
       <c r="F19" s="80"/>
     </row>
-    <row r="20" spans="1:6" ht="15.6" thickBot="1">
+    <row r="20" spans="1:6" ht="15.4" thickBot="1">
       <c r="A20" s="81" t="s">
         <v>733</v>
       </c>
@@ -5399,16 +5415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA98114-2501-4EF7-AF09-0FC113866AE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
@@ -5531,14 +5547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E50D85-45BE-43BD-8EEE-DE4DF7191B60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.6640625" style="1"/>
@@ -5547,7 +5563,7 @@
     <col min="6" max="6" width="34.33203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="46.95" customHeight="1">
+    <row r="1" spans="1:6" ht="47" customHeight="1">
       <c r="A1" s="111" t="s">
         <v>738</v>
       </c>
@@ -5685,7 +5701,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="79.2">
+    <row r="9" spans="1:6" ht="76.5">
       <c r="A9" s="109"/>
       <c r="B9" s="6" t="s">
         <v>3</v>
@@ -5723,7 +5739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39.6">
+    <row r="11" spans="1:6" ht="38.25">
       <c r="A11" s="112"/>
       <c r="B11" s="6" t="s">
         <v>3</v>
@@ -5761,7 +5777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39.6">
+    <row r="13" spans="1:6" ht="38.25">
       <c r="A13" s="110"/>
       <c r="B13" s="104" t="s">
         <v>3</v>
@@ -5779,7 +5795,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39.6">
+    <row r="14" spans="1:6" ht="38.25">
       <c r="A14" s="110"/>
       <c r="B14" s="6" t="s">
         <v>3</v>
@@ -5817,7 +5833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26.4">
+    <row r="16" spans="1:6" ht="25.5">
       <c r="A16" s="110"/>
       <c r="B16" s="6" t="s">
         <v>10</v>
@@ -6091,7 +6107,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="26.4">
+    <row r="31" spans="1:12" ht="25.5">
       <c r="A31" s="110"/>
       <c r="B31" s="17" t="s">
         <v>4</v>
@@ -6109,7 +6125,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="26.4">
+    <row r="32" spans="1:12" ht="25.5">
       <c r="A32" s="110"/>
       <c r="B32" s="17" t="s">
         <v>4</v>
@@ -6126,8 +6142,11 @@
       <c r="F32" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="26.4">
+      <c r="G32" s="137" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="25.5">
       <c r="A33" s="110"/>
       <c r="B33" s="17" t="s">
         <v>4</v>
@@ -6329,20 +6348,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920B052D-1130-4579-8DCD-D18586615F9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45.45" customHeight="1">
+    <row r="1" spans="1:6" ht="45.5" customHeight="1">
       <c r="A1" s="111" t="s">
         <v>739</v>
       </c>
@@ -6838,20 +6857,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A8365A-66C7-4E96-8C24-5C7B8139E778}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.45" customHeight="1">
+    <row r="1" spans="1:6" ht="42.5" customHeight="1">
       <c r="A1" s="111" t="s">
         <v>743</v>
       </c>
@@ -6975,7 +6994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39.6">
+    <row r="8" spans="1:6" ht="38.25">
       <c r="A8" s="110"/>
       <c r="B8" s="21" t="s">
         <v>4</v>
@@ -6993,7 +7012,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39.6">
+    <row r="9" spans="1:6" ht="38.25">
       <c r="A9" s="110"/>
       <c r="B9" s="21" t="s">
         <v>4</v>
@@ -7011,7 +7030,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.4">
+    <row r="10" spans="1:6" ht="25.5">
       <c r="A10" s="112"/>
       <c r="B10" s="21" t="s">
         <v>105</v>
@@ -7125,7 +7144,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26.4">
+    <row r="16" spans="1:6" ht="25.5">
       <c r="A16" s="110"/>
       <c r="B16" s="21" t="s">
         <v>131</v>
@@ -7163,7 +7182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="39.6">
+    <row r="18" spans="1:6" ht="38.25">
       <c r="A18" s="110"/>
       <c r="B18" s="21" t="s">
         <v>136</v>
@@ -7239,7 +7258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.4">
+    <row r="22" spans="1:6" ht="25.5">
       <c r="A22" s="110"/>
       <c r="B22" s="21" t="s">
         <v>143</v>
@@ -7353,20 +7372,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F97639-5499-4CB8-8C37-9AB97DD5CB65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="2" max="2" width="8.6640625" style="24"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1"/>
     <col min="6" max="6" width="63.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50.55" customHeight="1">
@@ -7418,7 +7437,7 @@
       <c r="F3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="128" t="s">
         <v>187</v>
       </c>
     </row>
@@ -7439,7 +7458,7 @@
       <c r="F4" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="118"/>
+      <c r="G4" s="125"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="110"/>
@@ -7458,7 +7477,7 @@
       <c r="F5" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="118"/>
+      <c r="G5" s="125"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="112"/>
@@ -7477,7 +7496,7 @@
       <c r="F6" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="119"/>
+      <c r="G6" s="126"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="110" t="s">
@@ -7498,11 +7517,11 @@
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="117" t="s">
+      <c r="G7" s="128" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.6">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="110"/>
       <c r="B8" s="23" t="s">
         <v>105</v>
@@ -7519,7 +7538,7 @@
       <c r="F8" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="118"/>
+      <c r="G8" s="125"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="110"/>
@@ -7538,7 +7557,7 @@
       <c r="F9" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="G9" s="118"/>
+      <c r="G9" s="125"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="112"/>
@@ -7557,7 +7576,7 @@
       <c r="F10" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="119"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="110" t="s">
@@ -7578,7 +7597,7 @@
       <c r="F11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="121" t="s">
+      <c r="G11" s="134" t="s">
         <v>189</v>
       </c>
     </row>
@@ -7599,7 +7618,7 @@
       <c r="F12" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="G12" s="122"/>
+      <c r="G12" s="135"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="110"/>
@@ -7618,9 +7637,9 @@
       <c r="F13" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="G13" s="122"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6">
+      <c r="G13" s="135"/>
+    </row>
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" s="112"/>
       <c r="B14" s="23" t="s">
         <v>105</v>
@@ -7637,7 +7656,7 @@
       <c r="F14" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="G14" s="123"/>
+      <c r="G14" s="136"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="110" t="s">
@@ -7658,7 +7677,7 @@
       <c r="F15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="121" t="s">
+      <c r="G15" s="134" t="s">
         <v>198</v>
       </c>
     </row>
@@ -7679,9 +7698,9 @@
       <c r="F16" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="G16" s="122"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6">
+      <c r="G16" s="135"/>
+    </row>
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="110"/>
       <c r="B17" s="23" t="s">
         <v>105</v>
@@ -7698,7 +7717,7 @@
       <c r="F17" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="G17" s="122"/>
+      <c r="G17" s="135"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="110"/>
@@ -7717,9 +7736,9 @@
       <c r="F18" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="122"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6">
+      <c r="G18" s="135"/>
+    </row>
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" s="112"/>
       <c r="B19" s="23" t="s">
         <v>105</v>
@@ -7736,7 +7755,7 @@
       <c r="F19" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="G19" s="123"/>
+      <c r="G19" s="136"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="110" t="s">
@@ -7757,7 +7776,7 @@
       <c r="F20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="121" t="s">
+      <c r="G20" s="134" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7778,9 +7797,9 @@
       <c r="F21" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="G21" s="122"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6">
+      <c r="G21" s="135"/>
+    </row>
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="110"/>
       <c r="B22" s="23" t="s">
         <v>4</v>
@@ -7797,7 +7816,7 @@
       <c r="F22" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="G22" s="123"/>
+      <c r="G22" s="136"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="110" t="s">
@@ -7818,11 +7837,11 @@
       <c r="F23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="120" t="s">
+      <c r="G23" s="133" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="110"/>
       <c r="B24" s="32" t="s">
         <v>213</v>
@@ -7839,7 +7858,7 @@
       <c r="F24" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="G24" s="120"/>
+      <c r="G24" s="133"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="110"/>
@@ -7858,9 +7877,9 @@
       <c r="F25" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="G25" s="120"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.6">
+      <c r="G25" s="133"/>
+    </row>
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="110"/>
       <c r="B26" s="32" t="s">
         <v>214</v>
@@ -7877,7 +7896,7 @@
       <c r="F26" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G26" s="120"/>
+      <c r="G26" s="133"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="110"/>
@@ -7896,7 +7915,7 @@
       <c r="F27" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="120"/>
+      <c r="G27" s="133"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="110"/>
@@ -7915,7 +7934,7 @@
       <c r="F28" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="G28" s="120"/>
+      <c r="G28" s="133"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="110"/>
@@ -7934,7 +7953,7 @@
       <c r="F29" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="G29" s="120"/>
+      <c r="G29" s="133"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="110"/>
@@ -7953,7 +7972,7 @@
       <c r="F30" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="120"/>
+      <c r="G30" s="133"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="110"/>
@@ -7972,7 +7991,7 @@
       <c r="F31" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="G31" s="120"/>
+      <c r="G31" s="133"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="110"/>
@@ -7991,10 +8010,10 @@
       <c r="F32" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="G32" s="120"/>
+      <c r="G32" s="133"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="127" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="23" t="s">
@@ -8012,10 +8031,10 @@
       <c r="F33" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="120"/>
+      <c r="G33" s="133"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="116"/>
+      <c r="A34" s="127"/>
       <c r="B34" s="23" t="s">
         <v>18</v>
       </c>
@@ -8031,10 +8050,10 @@
       <c r="F34" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="G34" s="120"/>
+      <c r="G34" s="133"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="116"/>
+      <c r="A35" s="127"/>
       <c r="B35" s="32" t="s">
         <v>245</v>
       </c>
@@ -8050,10 +8069,10 @@
       <c r="F35" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="G35" s="120"/>
+      <c r="G35" s="133"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="116"/>
+      <c r="A36" s="127"/>
       <c r="B36" s="32" t="s">
         <v>214</v>
       </c>
@@ -8069,10 +8088,10 @@
       <c r="F36" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="G36" s="120"/>
+      <c r="G36" s="133"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="116"/>
+      <c r="A37" s="127"/>
       <c r="B37" s="32" t="s">
         <v>246</v>
       </c>
@@ -8088,10 +8107,10 @@
       <c r="F37" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="G37" s="120"/>
+      <c r="G37" s="133"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="116"/>
+      <c r="A38" s="127"/>
       <c r="B38" s="32" t="s">
         <v>213</v>
       </c>
@@ -8107,10 +8126,10 @@
       <c r="F38" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="G38" s="120"/>
+      <c r="G38" s="133"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="116"/>
+      <c r="A39" s="127"/>
       <c r="B39" s="32" t="s">
         <v>213</v>
       </c>
@@ -8126,10 +8145,10 @@
       <c r="F39" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="G39" s="120"/>
+      <c r="G39" s="133"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="116"/>
+      <c r="A40" s="127"/>
       <c r="B40" s="32" t="s">
         <v>213</v>
       </c>
@@ -8145,10 +8164,10 @@
       <c r="F40" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="G40" s="120"/>
+      <c r="G40" s="133"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="116"/>
+      <c r="A41" s="127"/>
       <c r="B41" s="32" t="s">
         <v>214</v>
       </c>
@@ -8164,10 +8183,10 @@
       <c r="F41" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="G41" s="120"/>
+      <c r="G41" s="133"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="116"/>
+      <c r="A42" s="127"/>
       <c r="B42" s="32" t="s">
         <v>214</v>
       </c>
@@ -8183,10 +8202,10 @@
       <c r="F42" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="G42" s="120"/>
+      <c r="G42" s="133"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="116"/>
+      <c r="A43" s="127"/>
       <c r="B43" s="32" t="s">
         <v>214</v>
       </c>
@@ -8202,10 +8221,10 @@
       <c r="F43" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="G43" s="120"/>
+      <c r="G43" s="133"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="127" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="23" t="s">
@@ -8223,12 +8242,12 @@
       <c r="F44" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="117" t="s">
+      <c r="G44" s="128" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="116"/>
+      <c r="A45" s="127"/>
       <c r="B45" s="48" t="s">
         <v>213</v>
       </c>
@@ -8244,10 +8263,10 @@
       <c r="F45" s="50" t="s">
         <v>528</v>
       </c>
-      <c r="G45" s="118"/>
+      <c r="G45" s="125"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="116"/>
+      <c r="A46" s="127"/>
       <c r="B46" s="33" t="s">
         <v>213</v>
       </c>
@@ -8263,10 +8282,10 @@
       <c r="F46" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="G46" s="118"/>
+      <c r="G46" s="125"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="116"/>
+      <c r="A47" s="127"/>
       <c r="B47" s="33" t="s">
         <v>214</v>
       </c>
@@ -8282,10 +8301,10 @@
       <c r="F47" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="G47" s="118"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.6">
-      <c r="A48" s="116"/>
+      <c r="G47" s="125"/>
+    </row>
+    <row r="48" spans="1:7" ht="15">
+      <c r="A48" s="127"/>
       <c r="B48" s="34" t="s">
         <v>213</v>
       </c>
@@ -8301,10 +8320,10 @@
       <c r="F48" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="G48" s="118"/>
+      <c r="G48" s="125"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="116"/>
+      <c r="A49" s="127"/>
       <c r="B49" s="33" t="s">
         <v>213</v>
       </c>
@@ -8320,10 +8339,10 @@
       <c r="F49" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="G49" s="118"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.6">
-      <c r="A50" s="116"/>
+      <c r="G49" s="125"/>
+    </row>
+    <row r="50" spans="1:7" ht="15">
+      <c r="A50" s="127"/>
       <c r="B50" s="33" t="s">
         <v>213</v>
       </c>
@@ -8339,10 +8358,10 @@
       <c r="F50" s="28" t="s">
         <v>277</v>
       </c>
-      <c r="G50" s="118"/>
+      <c r="G50" s="125"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="116"/>
+      <c r="A51" s="127"/>
       <c r="B51" s="33" t="s">
         <v>213</v>
       </c>
@@ -8358,7 +8377,7 @@
       <c r="F51" s="28" t="s">
         <v>278</v>
       </c>
-      <c r="G51" s="119"/>
+      <c r="G51" s="126"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="124" t="s">
@@ -8379,12 +8398,12 @@
       <c r="F52" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G52" s="120" t="s">
+      <c r="G52" s="133" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="125"/>
+      <c r="A53" s="131"/>
       <c r="B53" s="35" t="s">
         <v>213</v>
       </c>
@@ -8400,10 +8419,10 @@
       <c r="F53" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="G53" s="120"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.6">
-      <c r="A54" s="125"/>
+      <c r="G53" s="133"/>
+    </row>
+    <row r="54" spans="1:7" ht="15">
+      <c r="A54" s="131"/>
       <c r="B54" s="35" t="s">
         <v>213</v>
       </c>
@@ -8419,10 +8438,10 @@
       <c r="F54" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="G54" s="120"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.6">
-      <c r="A55" s="125"/>
+      <c r="G54" s="133"/>
+    </row>
+    <row r="55" spans="1:7" ht="15">
+      <c r="A55" s="131"/>
       <c r="B55" s="35" t="s">
         <v>213</v>
       </c>
@@ -8438,10 +8457,10 @@
       <c r="F55" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="G55" s="120"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.6">
-      <c r="A56" s="125"/>
+      <c r="G55" s="133"/>
+    </row>
+    <row r="56" spans="1:7" ht="15">
+      <c r="A56" s="131"/>
       <c r="B56" s="35" t="s">
         <v>213</v>
       </c>
@@ -8457,10 +8476,10 @@
       <c r="F56" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="G56" s="120"/>
+      <c r="G56" s="133"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="125"/>
+      <c r="A57" s="131"/>
       <c r="B57" s="35" t="s">
         <v>298</v>
       </c>
@@ -8476,10 +8495,10 @@
       <c r="F57" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="G57" s="120"/>
+      <c r="G57" s="133"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="125"/>
+      <c r="A58" s="131"/>
       <c r="B58" s="35" t="s">
         <v>298</v>
       </c>
@@ -8495,10 +8514,10 @@
       <c r="F58" s="28" t="s">
         <v>297</v>
       </c>
-      <c r="G58" s="120"/>
+      <c r="G58" s="133"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="126"/>
+      <c r="A59" s="132"/>
       <c r="B59" s="35" t="s">
         <v>298</v>
       </c>
@@ -8514,10 +8533,10 @@
       <c r="F59" s="28" t="s">
         <v>297</v>
       </c>
-      <c r="G59" s="120"/>
+      <c r="G59" s="133"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="116" t="s">
+      <c r="A60" s="127" t="s">
         <v>23</v>
       </c>
       <c r="B60" s="23" t="s">
@@ -8535,12 +8554,12 @@
       <c r="F60" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G60" s="117" t="s">
+      <c r="G60" s="128" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="116"/>
+      <c r="A61" s="127"/>
       <c r="B61" s="32" t="s">
         <v>4</v>
       </c>
@@ -8556,10 +8575,10 @@
       <c r="F61" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="G61" s="118"/>
+      <c r="G61" s="125"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="116"/>
+      <c r="A62" s="127"/>
       <c r="B62" s="32" t="s">
         <v>4</v>
       </c>
@@ -8575,10 +8594,10 @@
       <c r="F62" s="28" t="s">
         <v>304</v>
       </c>
-      <c r="G62" s="119"/>
+      <c r="G62" s="126"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="116" t="s">
+      <c r="A63" s="127" t="s">
         <v>27</v>
       </c>
       <c r="B63" s="23" t="s">
@@ -8596,12 +8615,12 @@
       <c r="F63" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G63" s="120" t="s">
+      <c r="G63" s="133" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="116"/>
+      <c r="A64" s="127"/>
       <c r="B64" s="32" t="s">
         <v>4</v>
       </c>
@@ -8617,10 +8636,10 @@
       <c r="F64" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="G64" s="120"/>
+      <c r="G64" s="133"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="116"/>
+      <c r="A65" s="127"/>
       <c r="B65" s="32" t="s">
         <v>4</v>
       </c>
@@ -8636,10 +8655,10 @@
       <c r="F65" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="G65" s="120"/>
+      <c r="G65" s="133"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="116"/>
+      <c r="A66" s="127"/>
       <c r="B66" s="32" t="s">
         <v>3</v>
       </c>
@@ -8655,10 +8674,10 @@
       <c r="F66" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="G66" s="120"/>
+      <c r="G66" s="133"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="116"/>
+      <c r="A67" s="127"/>
       <c r="B67" s="32" t="s">
         <v>3</v>
       </c>
@@ -8674,10 +8693,10 @@
       <c r="F67" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="G67" s="120"/>
+      <c r="G67" s="133"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="116"/>
+      <c r="A68" s="127"/>
       <c r="B68" s="32" t="s">
         <v>3</v>
       </c>
@@ -8693,10 +8712,10 @@
       <c r="F68" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="G68" s="120"/>
+      <c r="G68" s="133"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="116" t="s">
+      <c r="A69" s="127" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="23" t="s">
@@ -8714,12 +8733,12 @@
       <c r="F69" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G69" s="120" t="s">
+      <c r="G69" s="133" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1">
-      <c r="A70" s="116"/>
+      <c r="A70" s="127"/>
       <c r="B70" s="32" t="s">
         <v>539</v>
       </c>
@@ -8735,10 +8754,10 @@
       <c r="F70" s="28" t="s">
         <v>533</v>
       </c>
-      <c r="G70" s="120"/>
+      <c r="G70" s="133"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="116" t="s">
+      <c r="A71" s="127" t="s">
         <v>78</v>
       </c>
       <c r="B71" s="23" t="s">
@@ -8756,10 +8775,10 @@
       <c r="F71" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="120"/>
+      <c r="G71" s="133"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="116"/>
+      <c r="A72" s="127"/>
       <c r="B72" s="32" t="s">
         <v>540</v>
       </c>
@@ -8775,10 +8794,10 @@
       <c r="F72" s="28" t="s">
         <v>535</v>
       </c>
-      <c r="G72" s="120"/>
+      <c r="G72" s="133"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="116" t="s">
+      <c r="A73" s="127" t="s">
         <v>79</v>
       </c>
       <c r="B73" s="23" t="s">
@@ -8793,17 +8812,17 @@
       <c r="F73" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G73" s="120"/>
+      <c r="G73" s="133"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="116"/>
-      <c r="B74" s="129" t="s">
+      <c r="A74" s="127"/>
+      <c r="B74" s="121" t="s">
         <v>918</v>
       </c>
       <c r="C74" s="108" t="s">
         <v>917</v>
       </c>
-      <c r="D74" s="131" t="s">
+      <c r="D74" s="116" t="s">
         <v>919</v>
       </c>
       <c r="E74" s="44" t="s">
@@ -8812,36 +8831,36 @@
       <c r="F74" s="45" t="s">
         <v>844</v>
       </c>
-      <c r="G74" s="120"/>
+      <c r="G74" s="133"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="116"/>
-      <c r="B75" s="134"/>
-      <c r="C75" s="134"/>
-      <c r="D75" s="132"/>
+      <c r="A75" s="127"/>
+      <c r="B75" s="119"/>
+      <c r="C75" s="119"/>
+      <c r="D75" s="117"/>
       <c r="E75" s="44" t="s">
         <v>915</v>
       </c>
       <c r="F75" s="45" t="s">
         <v>843</v>
       </c>
-      <c r="G75" s="120"/>
+      <c r="G75" s="133"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="116"/>
-      <c r="B76" s="130"/>
-      <c r="C76" s="130"/>
-      <c r="D76" s="133"/>
+      <c r="A76" s="127"/>
+      <c r="B76" s="120"/>
+      <c r="C76" s="120"/>
+      <c r="D76" s="118"/>
       <c r="E76" s="44" t="s">
         <v>914</v>
       </c>
       <c r="F76" s="45" t="s">
         <v>842</v>
       </c>
-      <c r="G76" s="120"/>
+      <c r="G76" s="133"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="116"/>
+      <c r="A77" s="127"/>
       <c r="B77" s="23"/>
       <c r="C77" s="97"/>
       <c r="E77" s="5" t="s">
@@ -8850,10 +8869,10 @@
       <c r="F77" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G77" s="120"/>
-    </row>
-    <row r="78" spans="1:7" ht="41.4">
-      <c r="A78" s="116"/>
+      <c r="G77" s="133"/>
+    </row>
+    <row r="78" spans="1:7" ht="41.65">
+      <c r="A78" s="127"/>
       <c r="B78" s="23" t="s">
         <v>213</v>
       </c>
@@ -8869,10 +8888,10 @@
       <c r="F78" s="57" t="s">
         <v>587</v>
       </c>
-      <c r="G78" s="120"/>
-    </row>
-    <row r="79" spans="1:7" ht="41.4">
-      <c r="A79" s="116"/>
+      <c r="G78" s="133"/>
+    </row>
+    <row r="79" spans="1:7" ht="41.65">
+      <c r="A79" s="127"/>
       <c r="B79" s="32" t="s">
         <v>4</v>
       </c>
@@ -8888,10 +8907,10 @@
       <c r="F79" s="57" t="s">
         <v>584</v>
       </c>
-      <c r="G79" s="120"/>
+      <c r="G79" s="133"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="116"/>
+      <c r="A80" s="127"/>
       <c r="B80" s="32"/>
       <c r="C80" s="9"/>
       <c r="D80" s="28"/>
@@ -8901,10 +8920,10 @@
       <c r="F80" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G80" s="120"/>
+      <c r="G80" s="133"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="116"/>
+      <c r="A81" s="127"/>
       <c r="B81" s="32" t="s">
         <v>4</v>
       </c>
@@ -8920,10 +8939,10 @@
       <c r="F81" s="28" t="s">
         <v>912</v>
       </c>
-      <c r="G81" s="120"/>
+      <c r="G81" s="133"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="116"/>
+      <c r="A82" s="127"/>
       <c r="B82" s="32" t="s">
         <v>4</v>
       </c>
@@ -8939,10 +8958,10 @@
       <c r="F82" s="28" t="s">
         <v>538</v>
       </c>
-      <c r="G82" s="120"/>
+      <c r="G82" s="133"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="116" t="s">
+      <c r="A83" s="127" t="s">
         <v>541</v>
       </c>
       <c r="B83" s="23" t="s">
@@ -8960,12 +8979,12 @@
       <c r="F83" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G83" s="120" t="s">
+      <c r="G83" s="133" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="116"/>
+      <c r="A84" s="127"/>
       <c r="B84" s="23" t="s">
         <v>4</v>
       </c>
@@ -8981,10 +9000,10 @@
       <c r="F84" s="28" t="s">
         <v>547</v>
       </c>
-      <c r="G84" s="120"/>
+      <c r="G84" s="133"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="116"/>
+      <c r="A85" s="127"/>
       <c r="B85" s="32" t="s">
         <v>4</v>
       </c>
@@ -9000,10 +9019,10 @@
       <c r="F85" s="28" t="s">
         <v>543</v>
       </c>
-      <c r="G85" s="120"/>
+      <c r="G85" s="133"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="116"/>
+      <c r="A86" s="127"/>
       <c r="B86" s="32" t="s">
         <v>545</v>
       </c>
@@ -9019,10 +9038,10 @@
       <c r="F86" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="G86" s="120"/>
+      <c r="G86" s="133"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="116" t="s">
+      <c r="A87" s="127" t="s">
         <v>549</v>
       </c>
       <c r="B87" s="23" t="s">
@@ -9040,13 +9059,13 @@
       <c r="F87" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G87" s="120" t="s">
+      <c r="G87" s="133" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="116"/>
-      <c r="B88" s="129" t="s">
+      <c r="A88" s="127"/>
+      <c r="B88" s="121" t="s">
         <v>298</v>
       </c>
       <c r="C88" s="108" t="s">
@@ -9061,36 +9080,36 @@
       <c r="F88" s="102" t="s">
         <v>926</v>
       </c>
-      <c r="G88" s="120"/>
+      <c r="G88" s="133"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="116"/>
-      <c r="B89" s="134"/>
-      <c r="C89" s="134"/>
-      <c r="D89" s="135"/>
+      <c r="A89" s="127"/>
+      <c r="B89" s="119"/>
+      <c r="C89" s="119"/>
+      <c r="D89" s="122"/>
       <c r="E89" s="101" t="s">
         <v>921</v>
       </c>
       <c r="F89" s="102" t="s">
         <v>920</v>
       </c>
-      <c r="G89" s="120"/>
-    </row>
-    <row r="90" spans="1:7" ht="27.6">
-      <c r="A90" s="116"/>
-      <c r="B90" s="130"/>
-      <c r="C90" s="130"/>
-      <c r="D90" s="136"/>
+      <c r="G89" s="133"/>
+    </row>
+    <row r="90" spans="1:7" ht="27.75">
+      <c r="A90" s="127"/>
+      <c r="B90" s="120"/>
+      <c r="C90" s="120"/>
+      <c r="D90" s="123"/>
       <c r="E90" s="9" t="s">
         <v>806</v>
       </c>
       <c r="F90" s="57" t="s">
         <v>922</v>
       </c>
-      <c r="G90" s="120"/>
+      <c r="G90" s="133"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="116"/>
+      <c r="A91" s="127"/>
       <c r="B91" s="32" t="s">
         <v>4</v>
       </c>
@@ -9106,10 +9125,10 @@
       <c r="F91" s="28" t="s">
         <v>553</v>
       </c>
-      <c r="G91" s="120"/>
+      <c r="G91" s="133"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="116"/>
+      <c r="A92" s="127"/>
       <c r="B92" s="32" t="s">
         <v>4</v>
       </c>
@@ -9125,10 +9144,10 @@
       <c r="F92" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="G92" s="120"/>
+      <c r="G92" s="133"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="116" t="s">
+      <c r="A93" s="127" t="s">
         <v>563</v>
       </c>
       <c r="B93" s="23" t="s">
@@ -9146,12 +9165,12 @@
       <c r="F93" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G93" s="117" t="s">
+      <c r="G93" s="128" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="116"/>
+      <c r="A94" s="127"/>
       <c r="B94" s="23"/>
       <c r="C94" s="104"/>
       <c r="D94" s="104"/>
@@ -9161,10 +9180,10 @@
       <c r="F94" s="45" t="s">
         <v>959</v>
       </c>
-      <c r="G94" s="118"/>
+      <c r="G94" s="125"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="116"/>
+      <c r="A95" s="127"/>
       <c r="B95" s="23"/>
       <c r="C95" s="104"/>
       <c r="D95" s="104"/>
@@ -9174,10 +9193,10 @@
       <c r="F95" s="45" t="s">
         <v>956</v>
       </c>
-      <c r="G95" s="118"/>
-    </row>
-    <row r="96" spans="1:7" ht="26.4">
-      <c r="A96" s="116"/>
+      <c r="G95" s="125"/>
+    </row>
+    <row r="96" spans="1:7" ht="25.5">
+      <c r="A96" s="127"/>
       <c r="B96" s="23" t="s">
         <v>105</v>
       </c>
@@ -9193,10 +9212,10 @@
       <c r="F96" s="19" t="s">
         <v>924</v>
       </c>
-      <c r="G96" s="118"/>
-    </row>
-    <row r="97" spans="1:7" ht="79.2">
-      <c r="A97" s="116"/>
+      <c r="G96" s="125"/>
+    </row>
+    <row r="97" spans="1:7" ht="76.5">
+      <c r="A97" s="127"/>
       <c r="B97" s="23" t="s">
         <v>4</v>
       </c>
@@ -9212,10 +9231,10 @@
       <c r="F97" s="19" t="s">
         <v>562</v>
       </c>
-      <c r="G97" s="118"/>
+      <c r="G97" s="125"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="116"/>
+      <c r="A98" s="127"/>
       <c r="B98" s="32" t="s">
         <v>4</v>
       </c>
@@ -9231,10 +9250,10 @@
       <c r="F98" s="28" t="s">
         <v>561</v>
       </c>
-      <c r="G98" s="118"/>
+      <c r="G98" s="125"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="116"/>
+      <c r="A99" s="127"/>
       <c r="B99" s="32" t="s">
         <v>4</v>
       </c>
@@ -9250,10 +9269,10 @@
       <c r="F99" s="28" t="s">
         <v>873</v>
       </c>
-      <c r="G99" s="118"/>
+      <c r="G99" s="125"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="116" t="s">
+      <c r="A100" s="127" t="s">
         <v>567</v>
       </c>
       <c r="B100" s="23" t="s">
@@ -9271,10 +9290,10 @@
       <c r="F100" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G100" s="118"/>
+      <c r="G100" s="125"/>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="116"/>
+      <c r="A101" s="127"/>
       <c r="B101" s="23" t="s">
         <v>884</v>
       </c>
@@ -9290,10 +9309,10 @@
       <c r="F101" s="53" t="s">
         <v>565</v>
       </c>
-      <c r="G101" s="118"/>
+      <c r="G101" s="125"/>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="116" t="s">
+      <c r="A102" s="127" t="s">
         <v>786</v>
       </c>
       <c r="B102" s="23" t="s">
@@ -9311,10 +9330,10 @@
       <c r="F102" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G102" s="118"/>
+      <c r="G102" s="125"/>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="116"/>
+      <c r="A103" s="127"/>
       <c r="B103" s="23" t="s">
         <v>885</v>
       </c>
@@ -9330,10 +9349,10 @@
       <c r="F103" s="53" t="s">
         <v>569</v>
       </c>
-      <c r="G103" s="118"/>
+      <c r="G103" s="125"/>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="116" t="s">
+      <c r="A104" s="127" t="s">
         <v>577</v>
       </c>
       <c r="B104" s="23" t="s">
@@ -9351,10 +9370,10 @@
       <c r="F104" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G104" s="118"/>
+      <c r="G104" s="125"/>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="116"/>
+      <c r="A105" s="127"/>
       <c r="B105" s="95"/>
       <c r="C105" s="92" t="s">
         <v>756</v>
@@ -9368,10 +9387,10 @@
       <c r="F105" s="45" t="s">
         <v>758</v>
       </c>
-      <c r="G105" s="118"/>
+      <c r="G105" s="125"/>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="116"/>
+      <c r="A106" s="127"/>
       <c r="B106" s="95"/>
       <c r="C106" s="92"/>
       <c r="D106" s="94"/>
@@ -9381,10 +9400,10 @@
       <c r="F106" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G106" s="118"/>
+      <c r="G106" s="125"/>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="116"/>
+      <c r="A107" s="127"/>
       <c r="B107" s="95" t="s">
         <v>213</v>
       </c>
@@ -9400,10 +9419,10 @@
       <c r="F107" s="45" t="s">
         <v>874</v>
       </c>
-      <c r="G107" s="118"/>
+      <c r="G107" s="125"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="116"/>
+      <c r="A108" s="127"/>
       <c r="B108" s="23" t="s">
         <v>880</v>
       </c>
@@ -9419,10 +9438,10 @@
       <c r="F108" s="53" t="s">
         <v>572</v>
       </c>
-      <c r="G108" s="118"/>
+      <c r="G108" s="125"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="116" t="s">
+      <c r="A109" s="127" t="s">
         <v>178</v>
       </c>
       <c r="B109" s="23" t="s">
@@ -9440,10 +9459,10 @@
       <c r="F109" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G109" s="118"/>
+      <c r="G109" s="125"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="116"/>
+      <c r="A110" s="127"/>
       <c r="B110" s="23" t="s">
         <v>881</v>
       </c>
@@ -9459,10 +9478,10 @@
       <c r="F110" s="53" t="s">
         <v>573</v>
       </c>
-      <c r="G110" s="119"/>
+      <c r="G110" s="126"/>
     </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="116" t="s">
+      <c r="A111" s="127" t="s">
         <v>580</v>
       </c>
       <c r="B111" s="23" t="s">
@@ -9480,19 +9499,19 @@
       <c r="F111" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G111" s="117" t="s">
+      <c r="G111" s="128" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="116"/>
-      <c r="B112" s="129" t="s">
+      <c r="A112" s="127"/>
+      <c r="B112" s="121" t="s">
         <v>751</v>
       </c>
       <c r="C112" s="108" t="s">
         <v>752</v>
       </c>
-      <c r="D112" s="127" t="s">
+      <c r="D112" s="129" t="s">
         <v>759</v>
       </c>
       <c r="E112" s="44" t="s">
@@ -9501,23 +9520,23 @@
       <c r="F112" s="45" t="s">
         <v>753</v>
       </c>
-      <c r="G112" s="118"/>
-    </row>
-    <row r="113" spans="1:7" ht="55.2">
-      <c r="A113" s="116"/>
-      <c r="B113" s="130"/>
-      <c r="C113" s="130"/>
-      <c r="D113" s="128"/>
+      <c r="G112" s="125"/>
+    </row>
+    <row r="113" spans="1:7" ht="55.5">
+      <c r="A113" s="127"/>
+      <c r="B113" s="120"/>
+      <c r="C113" s="120"/>
+      <c r="D113" s="130"/>
       <c r="E113" s="61" t="s">
         <v>749</v>
       </c>
       <c r="F113" s="55" t="s">
         <v>582</v>
       </c>
-      <c r="G113" s="118"/>
-    </row>
-    <row r="114" spans="1:7" ht="41.4">
-      <c r="A114" s="116"/>
+      <c r="G113" s="125"/>
+    </row>
+    <row r="114" spans="1:7" ht="41.65">
+      <c r="A114" s="127"/>
       <c r="B114" s="23" t="s">
         <v>4</v>
       </c>
@@ -9533,7 +9552,7 @@
       <c r="F114" s="55" t="s">
         <v>791</v>
       </c>
-      <c r="G114" s="118"/>
+      <c r="G114" s="125"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="124" t="s">
@@ -9552,12 +9571,12 @@
       <c r="F115" s="55" t="s">
         <v>773</v>
       </c>
-      <c r="G115" s="117" t="s">
+      <c r="G115" s="128" t="s">
         <v>886</v>
       </c>
     </row>
     <row r="116" spans="1:7">
-      <c r="A116" s="118"/>
+      <c r="A116" s="125"/>
       <c r="B116" s="23" t="s">
         <v>755</v>
       </c>
@@ -9573,10 +9592,10 @@
       <c r="F116" s="55" t="s">
         <v>770</v>
       </c>
-      <c r="G116" s="118"/>
+      <c r="G116" s="125"/>
     </row>
     <row r="117" spans="1:7">
-      <c r="A117" s="118"/>
+      <c r="A117" s="125"/>
       <c r="B117" s="23" t="s">
         <v>755</v>
       </c>
@@ -9592,10 +9611,10 @@
       <c r="F117" s="55" t="s">
         <v>767</v>
       </c>
-      <c r="G117" s="118"/>
+      <c r="G117" s="125"/>
     </row>
     <row r="118" spans="1:7">
-      <c r="A118" s="119"/>
+      <c r="A118" s="126"/>
       <c r="B118" s="23" t="s">
         <v>755</v>
       </c>
@@ -9611,10 +9630,10 @@
       <c r="F118" s="55" t="s">
         <v>764</v>
       </c>
-      <c r="G118" s="119"/>
+      <c r="G118" s="126"/>
     </row>
     <row r="119" spans="1:7">
-      <c r="A119" s="116" t="s">
+      <c r="A119" s="127" t="s">
         <v>597</v>
       </c>
       <c r="B119" s="23" t="s">
@@ -9632,12 +9651,12 @@
       <c r="F119" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G119" s="120" t="s">
+      <c r="G119" s="133" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="120" spans="1:7">
-      <c r="A120" s="116"/>
+      <c r="A120" s="127"/>
       <c r="B120" s="32" t="s">
         <v>105</v>
       </c>
@@ -9653,10 +9672,10 @@
       <c r="F120" s="28" t="s">
         <v>594</v>
       </c>
-      <c r="G120" s="120"/>
+      <c r="G120" s="133"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="116"/>
+      <c r="A121" s="127"/>
       <c r="B121" s="32" t="s">
         <v>545</v>
       </c>
@@ -9672,10 +9691,10 @@
       <c r="F121" s="28" t="s">
         <v>595</v>
       </c>
-      <c r="G121" s="120"/>
+      <c r="G121" s="133"/>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="116" t="s">
+      <c r="A122" s="127" t="s">
         <v>598</v>
       </c>
       <c r="B122" s="23" t="s">
@@ -9693,12 +9712,12 @@
       <c r="F122" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G122" s="117" t="s">
+      <c r="G122" s="128" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="116"/>
+      <c r="A123" s="127"/>
       <c r="B123" s="32" t="s">
         <v>604</v>
       </c>
@@ -9714,10 +9733,10 @@
       <c r="F123" s="28" t="s">
         <v>606</v>
       </c>
-      <c r="G123" s="118"/>
+      <c r="G123" s="125"/>
     </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="116"/>
+      <c r="A124" s="127"/>
       <c r="B124" s="32" t="s">
         <v>604</v>
       </c>
@@ -9733,10 +9752,10 @@
       <c r="F124" s="28" t="s">
         <v>608</v>
       </c>
-      <c r="G124" s="118"/>
+      <c r="G124" s="125"/>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="116"/>
+      <c r="A125" s="127"/>
       <c r="B125" s="32" t="s">
         <v>601</v>
       </c>
@@ -9752,10 +9771,10 @@
       <c r="F125" s="28" t="s">
         <v>610</v>
       </c>
-      <c r="G125" s="118"/>
+      <c r="G125" s="125"/>
     </row>
     <row r="126" spans="1:7">
-      <c r="A126" s="116"/>
+      <c r="A126" s="127"/>
       <c r="B126" s="32" t="s">
         <v>603</v>
       </c>
@@ -9771,10 +9790,10 @@
       <c r="F126" s="28" t="s">
         <v>613</v>
       </c>
-      <c r="G126" s="118"/>
+      <c r="G126" s="125"/>
     </row>
     <row r="127" spans="1:7">
-      <c r="A127" s="116"/>
+      <c r="A127" s="127"/>
       <c r="B127" s="32" t="s">
         <v>602</v>
       </c>
@@ -9790,10 +9809,10 @@
       <c r="F127" s="28" t="s">
         <v>615</v>
       </c>
-      <c r="G127" s="118"/>
+      <c r="G127" s="125"/>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="116"/>
+      <c r="A128" s="127"/>
       <c r="B128" s="32" t="s">
         <v>602</v>
       </c>
@@ -9809,10 +9828,10 @@
       <c r="F128" s="28" t="s">
         <v>617</v>
       </c>
-      <c r="G128" s="118"/>
+      <c r="G128" s="125"/>
     </row>
     <row r="129" spans="1:7">
-      <c r="A129" s="116"/>
+      <c r="A129" s="127"/>
       <c r="B129" s="32" t="s">
         <v>601</v>
       </c>
@@ -9828,10 +9847,10 @@
       <c r="F129" s="28" t="s">
         <v>619</v>
       </c>
-      <c r="G129" s="118"/>
+      <c r="G129" s="125"/>
     </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="116"/>
+      <c r="A130" s="127"/>
       <c r="B130" s="32" t="s">
         <v>600</v>
       </c>
@@ -9847,10 +9866,10 @@
       <c r="F130" s="28" t="s">
         <v>621</v>
       </c>
-      <c r="G130" s="119"/>
+      <c r="G130" s="126"/>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="116" t="s">
+      <c r="A131" s="127" t="s">
         <v>887</v>
       </c>
       <c r="B131" s="23" t="s">
@@ -9868,12 +9887,12 @@
       <c r="F131" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G131" s="117" t="s">
+      <c r="G131" s="128" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="132" spans="1:7">
-      <c r="A132" s="116"/>
+      <c r="A132" s="127"/>
       <c r="B132" s="32"/>
       <c r="C132" s="9" t="s">
         <v>0</v>
@@ -9887,10 +9906,10 @@
       <c r="F132" s="28" t="s">
         <v>893</v>
       </c>
-      <c r="G132" s="118"/>
+      <c r="G132" s="125"/>
     </row>
     <row r="133" spans="1:7">
-      <c r="A133" s="116" t="s">
+      <c r="A133" s="127" t="s">
         <v>890</v>
       </c>
       <c r="B133" s="23" t="s">
@@ -9908,10 +9927,10 @@
       <c r="F133" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G133" s="118"/>
+      <c r="G133" s="125"/>
     </row>
     <row r="134" spans="1:7">
-      <c r="A134" s="116"/>
+      <c r="A134" s="127"/>
       <c r="B134" s="32"/>
       <c r="C134" s="9" t="s">
         <v>0</v>
@@ -9925,10 +9944,10 @@
       <c r="F134" s="28" t="s">
         <v>892</v>
       </c>
-      <c r="G134" s="118"/>
+      <c r="G134" s="125"/>
     </row>
     <row r="135" spans="1:7">
-      <c r="A135" s="116" t="s">
+      <c r="A135" s="127" t="s">
         <v>896</v>
       </c>
       <c r="B135" s="23" t="s">
@@ -9946,10 +9965,10 @@
       <c r="F135" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G135" s="118"/>
+      <c r="G135" s="125"/>
     </row>
     <row r="136" spans="1:7">
-      <c r="A136" s="116"/>
+      <c r="A136" s="127"/>
       <c r="B136" s="32"/>
       <c r="C136" s="9" t="s">
         <v>0</v>
@@ -9963,10 +9982,10 @@
       <c r="F136" s="28" t="s">
         <v>895</v>
       </c>
-      <c r="G136" s="118"/>
+      <c r="G136" s="125"/>
     </row>
     <row r="137" spans="1:7">
-      <c r="A137" s="116" t="s">
+      <c r="A137" s="127" t="s">
         <v>897</v>
       </c>
       <c r="B137" s="23" t="s">
@@ -9984,10 +10003,10 @@
       <c r="F137" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G137" s="118"/>
+      <c r="G137" s="125"/>
     </row>
     <row r="138" spans="1:7">
-      <c r="A138" s="116"/>
+      <c r="A138" s="127"/>
       <c r="B138" s="23"/>
       <c r="C138" s="9" t="s">
         <v>0</v>
@@ -10001,10 +10020,10 @@
       <c r="F138" s="28" t="s">
         <v>902</v>
       </c>
-      <c r="G138" s="118"/>
+      <c r="G138" s="125"/>
     </row>
     <row r="139" spans="1:7">
-      <c r="A139" s="116"/>
+      <c r="A139" s="127"/>
       <c r="B139" s="23"/>
       <c r="C139" s="93"/>
       <c r="D139" s="93"/>
@@ -10014,10 +10033,10 @@
       <c r="F139" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G139" s="118"/>
+      <c r="G139" s="125"/>
     </row>
     <row r="140" spans="1:7">
-      <c r="A140" s="116"/>
+      <c r="A140" s="127"/>
       <c r="B140" s="32"/>
       <c r="C140" s="9" t="s">
         <v>0</v>
@@ -10031,10 +10050,10 @@
       <c r="F140" s="28" t="s">
         <v>899</v>
       </c>
-      <c r="G140" s="118"/>
+      <c r="G140" s="125"/>
     </row>
     <row r="141" spans="1:7">
-      <c r="A141" s="116" t="s">
+      <c r="A141" s="127" t="s">
         <v>903</v>
       </c>
       <c r="B141" s="23" t="s">
@@ -10052,10 +10071,10 @@
       <c r="F141" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G141" s="118"/>
+      <c r="G141" s="125"/>
     </row>
     <row r="142" spans="1:7">
-      <c r="A142" s="116"/>
+      <c r="A142" s="127"/>
       <c r="B142" s="23"/>
       <c r="C142" s="9" t="s">
         <v>0</v>
@@ -10069,10 +10088,10 @@
       <c r="F142" s="28" t="s">
         <v>906</v>
       </c>
-      <c r="G142" s="118"/>
+      <c r="G142" s="125"/>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" s="116"/>
+      <c r="A143" s="127"/>
       <c r="B143" s="23"/>
       <c r="C143" s="93"/>
       <c r="D143" s="93"/>
@@ -10082,10 +10101,10 @@
       <c r="F143" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G143" s="118"/>
+      <c r="G143" s="125"/>
     </row>
     <row r="144" spans="1:7">
-      <c r="A144" s="116"/>
+      <c r="A144" s="127"/>
       <c r="B144" s="32"/>
       <c r="C144" s="9" t="s">
         <v>0</v>
@@ -10099,47 +10118,16 @@
       <c r="F144" s="28" t="s">
         <v>907</v>
       </c>
-      <c r="G144" s="119"/>
+      <c r="G144" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="A93:A99"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="G93:G110"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="G115:G118"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A43"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A59"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="G63:G68"/>
-    <mergeCell ref="G60:G62"/>
-    <mergeCell ref="G52:G59"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="A137:A140"/>
+    <mergeCell ref="A141:A144"/>
+    <mergeCell ref="G131:G144"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
     <mergeCell ref="A122:A130"/>
     <mergeCell ref="G122:G130"/>
     <mergeCell ref="G23:G43"/>
@@ -10156,12 +10144,43 @@
     <mergeCell ref="G87:G92"/>
     <mergeCell ref="G44:G51"/>
     <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A137:A140"/>
-    <mergeCell ref="A141:A144"/>
-    <mergeCell ref="G131:G144"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="G63:G68"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="G52:G59"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="A93:A99"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="G93:G110"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="G115:G118"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B88:B90"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10170,14 +10189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28D0906-052D-43FD-A4BB-226D0BB88B0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
@@ -10251,7 +10270,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="39.6">
+    <row r="5" spans="1:6" ht="38.25">
       <c r="A5" s="110"/>
       <c r="B5" s="38" t="s">
         <v>4</v>
@@ -10433,7 +10452,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="132">
+    <row r="15" spans="1:6" ht="127.5">
       <c r="A15" s="112"/>
       <c r="B15" s="38" t="s">
         <v>340</v>
@@ -10547,7 +10566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="52.8">
+    <row r="21" spans="1:6" ht="51">
       <c r="A21" s="113"/>
       <c r="B21" s="38" t="s">
         <v>4</v>
@@ -10693,7 +10712,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="105.6">
+    <row r="29" spans="1:6" ht="102">
       <c r="A29" s="113"/>
       <c r="B29" s="38" t="s">
         <v>4</v>
@@ -10729,7 +10748,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="118.8">
+    <row r="31" spans="1:6" ht="114.75">
       <c r="A31" s="109"/>
       <c r="B31" s="38" t="s">
         <v>4</v>
@@ -10853,7 +10872,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="96.6">
+    <row r="38" spans="1:6" ht="83.25">
       <c r="A38" s="113"/>
       <c r="B38" s="86" t="s">
         <v>26</v>
@@ -10909,16 +10928,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9074A8-11E0-48D9-822A-54D3CEF7052B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
@@ -11090,10 +11109,10 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="134"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="44" t="s">
         <v>832</v>
       </c>
@@ -11102,10 +11121,10 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="134"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
+      <c r="A11" s="119"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="44" t="s">
         <v>830</v>
       </c>
@@ -11114,10 +11133,10 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="134"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
+      <c r="A12" s="119"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="44" t="s">
         <v>828</v>
       </c>
@@ -11126,10 +11145,10 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="134"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
+      <c r="A13" s="119"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
       <c r="E13" s="44" t="s">
         <v>826</v>
       </c>
@@ -11138,10 +11157,10 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="134"/>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
+      <c r="A14" s="119"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
       <c r="E14" s="44" t="s">
         <v>824</v>
       </c>
@@ -11150,10 +11169,10 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="134"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
+      <c r="A15" s="119"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
       <c r="E15" s="44" t="s">
         <v>822</v>
       </c>
@@ -11162,10 +11181,10 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="134"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
       <c r="E16" s="44" t="s">
         <v>820</v>
       </c>
@@ -11174,10 +11193,10 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="134"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
       <c r="E17" s="44" t="s">
         <v>818</v>
       </c>
@@ -11186,10 +11205,10 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="134"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
+      <c r="A18" s="119"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
       <c r="E18" s="44" t="s">
         <v>816</v>
       </c>
@@ -11198,10 +11217,10 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="134"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
+      <c r="A19" s="119"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
       <c r="E19" s="44" t="s">
         <v>814</v>
       </c>
@@ -11210,10 +11229,10 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="134"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
+      <c r="A20" s="119"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
       <c r="E20" s="44" t="s">
         <v>812</v>
       </c>
@@ -11222,10 +11241,10 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="134"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
+      <c r="A21" s="119"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
       <c r="E21" s="44" t="s">
         <v>810</v>
       </c>
@@ -11234,10 +11253,10 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="134"/>
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="134"/>
+      <c r="A22" s="119"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
       <c r="E22" s="44" t="s">
         <v>808</v>
       </c>
@@ -11246,10 +11265,10 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="134"/>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
+      <c r="A23" s="119"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
       <c r="E23" s="44" t="s">
         <v>806</v>
       </c>
@@ -11258,10 +11277,10 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="130"/>
-      <c r="B24" s="130"/>
-      <c r="C24" s="130"/>
-      <c r="D24" s="130"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
       <c r="E24" s="44" t="s">
         <v>804</v>
       </c>
@@ -11290,10 +11309,10 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="134"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
+      <c r="A26" s="119"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
       <c r="E26" s="44" t="s">
         <v>853</v>
       </c>
@@ -11302,10 +11321,10 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="134"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
+      <c r="A27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
       <c r="E27" s="44" t="s">
         <v>851</v>
       </c>
@@ -11314,10 +11333,10 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="134"/>
-      <c r="B28" s="134"/>
-      <c r="C28" s="134"/>
-      <c r="D28" s="134"/>
+      <c r="A28" s="119"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
       <c r="E28" s="44" t="s">
         <v>849</v>
       </c>
@@ -11326,10 +11345,10 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="134"/>
-      <c r="B29" s="134"/>
-      <c r="C29" s="134"/>
-      <c r="D29" s="134"/>
+      <c r="A29" s="119"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
       <c r="E29" s="44" t="s">
         <v>847</v>
       </c>
@@ -11338,10 +11357,10 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="134"/>
-      <c r="B30" s="134"/>
-      <c r="C30" s="134"/>
-      <c r="D30" s="134"/>
+      <c r="A30" s="119"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
       <c r="E30" s="44" t="s">
         <v>845</v>
       </c>
@@ -11350,10 +11369,10 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="134"/>
-      <c r="B31" s="134"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="134"/>
+      <c r="A31" s="119"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="119"/>
       <c r="E31" s="98" t="s">
         <v>818</v>
       </c>
@@ -11362,10 +11381,10 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="134"/>
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
+      <c r="A32" s="119"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="119"/>
       <c r="E32" s="98" t="s">
         <v>816</v>
       </c>
@@ -11374,10 +11393,10 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="134"/>
-      <c r="B33" s="134"/>
-      <c r="C33" s="134"/>
-      <c r="D33" s="134"/>
+      <c r="A33" s="119"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="119"/>
       <c r="E33" s="98" t="s">
         <v>814</v>
       </c>
@@ -11386,10 +11405,10 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="134"/>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
+      <c r="A34" s="119"/>
+      <c r="B34" s="119"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
       <c r="E34" s="44" t="s">
         <v>812</v>
       </c>
@@ -11398,10 +11417,10 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="134"/>
-      <c r="B35" s="134"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="134"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="119"/>
       <c r="E35" s="44" t="s">
         <v>810</v>
       </c>
@@ -11410,10 +11429,10 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="134"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
+      <c r="A36" s="119"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="119"/>
       <c r="E36" s="44" t="s">
         <v>808</v>
       </c>
@@ -11422,10 +11441,10 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="134"/>
-      <c r="B37" s="134"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
+      <c r="A37" s="119"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
       <c r="E37" s="44" t="s">
         <v>806</v>
       </c>
@@ -11434,10 +11453,10 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="130"/>
-      <c r="B38" s="130"/>
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
+      <c r="A38" s="120"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
       <c r="E38" s="44" t="s">
         <v>804</v>
       </c>
@@ -11644,9 +11663,9 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="13.05" customHeight="1">
-      <c r="A49" s="134"/>
-      <c r="B49" s="134"/>
-      <c r="C49" s="134"/>
+      <c r="A49" s="119"/>
+      <c r="B49" s="119"/>
+      <c r="C49" s="119"/>
       <c r="D49" s="108" t="s">
         <v>859</v>
       </c>
@@ -11658,10 +11677,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="13.05" customHeight="1">
-      <c r="A50" s="130"/>
-      <c r="B50" s="130"/>
-      <c r="C50" s="130"/>
-      <c r="D50" s="130"/>
+      <c r="A50" s="120"/>
+      <c r="B50" s="120"/>
+      <c r="C50" s="120"/>
+      <c r="D50" s="120"/>
       <c r="E50" s="44" t="s">
         <v>497</v>
       </c>
@@ -11688,9 +11707,9 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="13.05" customHeight="1">
-      <c r="A52" s="130"/>
-      <c r="B52" s="130"/>
-      <c r="C52" s="130"/>
+      <c r="A52" s="120"/>
+      <c r="B52" s="120"/>
+      <c r="C52" s="120"/>
       <c r="D52" s="93"/>
       <c r="E52" s="44" t="s">
         <v>864</v>
@@ -11797,7 +11816,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="113"/>
-      <c r="B58" s="134"/>
+      <c r="B58" s="119"/>
       <c r="C58" s="108" t="s">
         <v>28</v>
       </c>
@@ -11813,9 +11832,9 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="113"/>
-      <c r="B59" s="134"/>
-      <c r="C59" s="118"/>
-      <c r="D59" s="134"/>
+      <c r="B59" s="119"/>
+      <c r="C59" s="125"/>
+      <c r="D59" s="119"/>
       <c r="E59" s="93" t="s">
         <v>43</v>
       </c>
@@ -11825,9 +11844,9 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="113"/>
-      <c r="B60" s="134"/>
-      <c r="C60" s="118"/>
-      <c r="D60" s="134"/>
+      <c r="B60" s="119"/>
+      <c r="C60" s="125"/>
+      <c r="D60" s="119"/>
       <c r="E60" s="93" t="s">
         <v>42</v>
       </c>
@@ -11837,9 +11856,9 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="113"/>
-      <c r="B61" s="134"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="134"/>
+      <c r="B61" s="119"/>
+      <c r="C61" s="125"/>
+      <c r="D61" s="119"/>
       <c r="E61" s="93" t="s">
         <v>41</v>
       </c>
@@ -11849,9 +11868,9 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="109"/>
-      <c r="B62" s="130"/>
-      <c r="C62" s="119"/>
-      <c r="D62" s="130"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="126"/>
+      <c r="D62" s="120"/>
       <c r="E62" s="43" t="s">
         <v>38</v>
       </c>
@@ -12234,7 +12253,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="13.05" customHeight="1">
-      <c r="A84" s="130"/>
+      <c r="A84" s="120"/>
       <c r="B84" s="60" t="s">
         <v>4</v>
       </c>
@@ -12253,13 +12272,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D58:D62"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="B57:B62"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A7"/>
@@ -12276,13 +12295,13 @@
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D58:D62"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A62"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12291,16 +12310,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5462A84-5583-420E-A5C1-7ED4CC9711D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
@@ -13231,16 +13250,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D8D7B2-3DC2-4B4A-B1C5-224E4D25B711}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
@@ -13293,7 +13312,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.4">
+    <row r="4" spans="1:6" ht="25.5">
       <c r="A4" s="110"/>
       <c r="B4" s="43" t="s">
         <v>4</v>
@@ -13311,7 +13330,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="39.6">
+    <row r="5" spans="1:6" ht="38.25">
       <c r="A5" s="110"/>
       <c r="B5" s="43" t="s">
         <v>4</v>

</xml_diff>